<commit_message>
Added support for Excel master/secondary extracts
</commit_message>
<xml_diff>
--- a/MyDeptApp/20161229/MyDeptApp_FamilyNameCheck.xlsx
+++ b/MyDeptApp/20161229/MyDeptApp_FamilyNameCheck.xlsx
@@ -459,7 +459,7 @@
     <row r="2">
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -480,7 +480,7 @@
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="n">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="n">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -543,7 +543,7 @@
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="n">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -564,7 +564,7 @@
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="n">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="n">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="n">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -627,7 +627,7 @@
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="n">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -648,7 +648,7 @@
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="n">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
     <row r="12">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="n">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -690,7 +690,7 @@
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
     <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="n">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -732,7 +732,7 @@
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="n">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="n">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
     <row r="17">
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="n">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -795,7 +795,7 @@
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="n">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -816,7 +816,7 @@
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="n">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="n">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="n">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="n">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -900,7 +900,7 @@
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="n">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -921,7 +921,7 @@
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="n">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="n">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -963,7 +963,7 @@
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="n">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="n">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
     <row r="28">
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="n">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
     <row r="29">
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="n">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1047,7 +1047,7 @@
     <row r="30">
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="n">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1068,7 +1068,7 @@
     <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="n">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
     <row r="32">
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="n">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="n">
-        <v>1793</v>
+        <v>1791</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>

</xml_diff>